<commit_message>
modified billing utilization,trainings and travels
</commit_message>
<xml_diff>
--- a/Content/UploadedFiles/EmployeeBillingUtilization.xlsx
+++ b/Content/UploadedFiles/EmployeeBillingUtilization.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>Employee Name</t>
   </si>
@@ -40,7 +40,13 @@
     <t xml:space="preserve">Utilization on self </t>
   </si>
   <si>
-    <t>test</t>
+    <t>sdasa</t>
+  </si>
+  <si>
+    <t>ase</t>
+  </si>
+  <si>
+    <t>Frank Warnakula</t>
   </si>
 </sst>
 </file>
@@ -84,17 +90,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -399,10 +404,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -448,25 +453,74 @@
         <v>8</v>
       </c>
       <c r="B2" s="3">
-        <v>42257</v>
+        <v>42005</v>
       </c>
       <c r="C2" s="3">
-        <v>42257</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2">
-        <v>42</v>
+        <v>42369</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="4">
+        <v>8.5599999999999996E-2</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0.20200000000000001</v>
+      </c>
+      <c r="G2" s="4">
+        <v>1</v>
+      </c>
+      <c r="H2" s="5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="3">
+        <v>42006</v>
+      </c>
+      <c r="C3" s="3">
+        <v>42370</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="4">
+        <v>8.5599999999999996E-2</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0.20200000000000001</v>
+      </c>
+      <c r="G3" s="4">
+        <v>1</v>
+      </c>
+      <c r="H3" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="3">
+        <v>42006</v>
+      </c>
+      <c r="C4" s="3">
+        <v>42370</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="4">
+        <v>5.2600000000000001E-2</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0.125</v>
+      </c>
+      <c r="G4" s="4">
+        <v>1</v>
+      </c>
+      <c r="H4" s="6">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>